<commit_message>
primera version LSA Y TFIDF
</commit_message>
<xml_diff>
--- a/results/Clusters/10/ClusterDf_10.xlsx
+++ b/results/Clusters/10/ClusterDf_10.xlsx
@@ -11,21 +11,17 @@
     <sheet name="Cluster1" sheetId="2" r:id="rId2"/>
     <sheet name="Cluster2" sheetId="3" r:id="rId3"/>
     <sheet name="Cluster3" sheetId="4" r:id="rId4"/>
-    <sheet name="Cluster4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>clusters</t>
   </si>
   <si>
-    <t>Topic_0</t>
-  </si>
-  <si>
     <t>Topic_1</t>
   </si>
   <si>
@@ -71,13 +67,31 @@
     <t>Topic_15</t>
   </si>
   <si>
+    <t>Topic_16</t>
+  </si>
+  <si>
+    <t>Topic_17</t>
+  </si>
+  <si>
+    <t>Topic_18</t>
+  </si>
+  <si>
+    <t>Topic_19</t>
+  </si>
+  <si>
+    <t>antena3_2019 09 17_morning_new</t>
+  </si>
+  <si>
+    <t>antena3_2019 09 17_afternoon_new</t>
+  </si>
+  <si>
     <t>antena3_2019 09 16_morning_new</t>
   </si>
   <si>
-    <t>antena3_2019 09 17_morning_new</t>
-  </si>
-  <si>
-    <t>antena3_2019 09 17_afternoon_new</t>
+    <t>antena3_2019 09 18_morning_new</t>
+  </si>
+  <si>
+    <t>antena3_2019 09 14_morning_new</t>
   </si>
   <si>
     <t>antena3_2019 09 14_afternoon_new</t>
@@ -86,19 +100,13 @@
     <t>antena3_2019 09 15_morning_new</t>
   </si>
   <si>
-    <t>antena3_2019 09 14_morning_new</t>
-  </si>
-  <si>
     <t>antena3_2019 09 15_afternoon_new</t>
   </si>
   <si>
+    <t>antena3_2019 09 18_afternoon_new</t>
+  </si>
+  <si>
     <t>antena3_2019 09 16_afternoon_new</t>
-  </si>
-  <si>
-    <t>antena3_2019 09 18_morning_new</t>
-  </si>
-  <si>
-    <t>antena3_2019 09 18_afternoon_new</t>
   </si>
 </sst>
 </file>
@@ -456,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,10 +522,19 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -541,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.428</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -568,12 +585,21 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0.992</v>
+        <v>0.5649999999999999</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -597,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.262</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -624,63 +650,16 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0.733</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
         <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -690,13 +669,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,10 +727,19 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -775,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -793,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.988</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -804,10 +792,19 @@
       <c r="R2">
         <v>0</v>
       </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -831,26 +828,26 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
         <v>0</v>
       </c>
@@ -858,6 +855,15 @@
         <v>0</v>
       </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>0</v>
       </c>
     </row>
@@ -868,13 +874,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,10 +932,19 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -953,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.958</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -968,13 +983,13 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="O2">
-        <v>0.913</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -982,10 +997,19 @@
       <c r="R2">
         <v>0</v>
       </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1009,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.123</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1030,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.877</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1038,10 +1062,19 @@
       <c r="R3">
         <v>0</v>
       </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1065,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.716</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1086,12 +1119,151 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.284</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.533</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.467</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0.736</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.234</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0.014</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.015</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>0</v>
       </c>
     </row>
@@ -1102,13 +1274,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,10 +1332,19 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1187,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.207</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1199,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1211,131 +1392,18 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.792</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:18">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>0</v>
       </c>
     </row>

</xml_diff>